<commit_message>
V1.3 Color Display in Excel
</commit_message>
<xml_diff>
--- a/Balanced-Motor-Matrix.xlsx
+++ b/Balanced-Motor-Matrix.xlsx
@@ -26,12 +26,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +52,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,7 +522,7 @@
       <c r="B4" t="b">
         <v>0</v>
       </c>
-      <c r="C4" t="b">
+      <c r="C4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="b">
@@ -602,13 +609,13 @@
       <c r="B7" t="b">
         <v>0</v>
       </c>
-      <c r="C7" t="b">
+      <c r="C7" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
-      <c r="E7" t="b">
+      <c r="E7" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F7" t="b">
@@ -617,7 +624,7 @@
       <c r="G7" t="b">
         <v>0</v>
       </c>
-      <c r="H7" t="b">
+      <c r="H7" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I7" t="b">
@@ -689,22 +696,22 @@
       <c r="B10" t="b">
         <v>0</v>
       </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" t="b">
+      <c r="C10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I10" t="b">
@@ -776,22 +783,22 @@
       <c r="B13" t="b">
         <v>0</v>
       </c>
-      <c r="C13" t="b">
+      <c r="C13" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
       </c>
-      <c r="E13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" t="b">
+      <c r="E13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G13" t="b">
         <v>0</v>
       </c>
-      <c r="H13" t="b">
+      <c r="H13" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I13" t="b">
@@ -863,22 +870,22 @@
       <c r="B16" t="b">
         <v>0</v>
       </c>
-      <c r="C16" t="b">
+      <c r="C16" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
       </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="b">
+      <c r="E16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
       </c>
-      <c r="H16" t="b">
+      <c r="H16" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I16" t="b">
@@ -950,22 +957,22 @@
       <c r="B19" t="b">
         <v>0</v>
       </c>
-      <c r="C19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" t="b">
-        <v>1</v>
-      </c>
-      <c r="G19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" t="b">
+      <c r="C19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I19" t="b">
@@ -1037,22 +1044,22 @@
       <c r="B22" t="b">
         <v>0</v>
       </c>
-      <c r="C22" t="b">
+      <c r="C22" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
       </c>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" t="b">
+      <c r="E22" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G22" t="b">
         <v>0</v>
       </c>
-      <c r="H22" t="b">
+      <c r="H22" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I22" t="b">
@@ -1124,22 +1131,22 @@
       <c r="B25" t="b">
         <v>0</v>
       </c>
-      <c r="C25" t="b">
+      <c r="C25" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
       </c>
-      <c r="E25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" t="b">
+      <c r="E25" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
       </c>
-      <c r="H25" t="b">
+      <c r="H25" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I25" t="b">
@@ -1211,22 +1218,22 @@
       <c r="B28" t="b">
         <v>0</v>
       </c>
-      <c r="C28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G28" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" t="b">
+      <c r="C28" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I28" t="b">
@@ -1298,22 +1305,22 @@
       <c r="B31" t="b">
         <v>0</v>
       </c>
-      <c r="C31" t="b">
+      <c r="C31" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
       </c>
-      <c r="E31" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" t="b">
+      <c r="E31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G31" t="b">
         <v>0</v>
       </c>
-      <c r="H31" t="b">
+      <c r="H31" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I31" t="b">
@@ -1385,22 +1392,22 @@
       <c r="B34" t="b">
         <v>0</v>
       </c>
-      <c r="C34" t="b">
+      <c r="C34" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
       </c>
-      <c r="E34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" t="b">
+      <c r="E34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G34" t="b">
         <v>0</v>
       </c>
-      <c r="H34" t="b">
+      <c r="H34" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I34" t="b">
@@ -1472,22 +1479,22 @@
       <c r="B37" t="b">
         <v>0</v>
       </c>
-      <c r="C37" t="b">
-        <v>1</v>
-      </c>
-      <c r="D37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" t="b">
+      <c r="C37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I37" t="b">
@@ -1559,22 +1566,22 @@
       <c r="B40" t="b">
         <v>0</v>
       </c>
-      <c r="C40" t="b">
+      <c r="C40" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
       </c>
-      <c r="E40" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" t="b">
+      <c r="E40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G40" t="b">
         <v>0</v>
       </c>
-      <c r="H40" t="b">
+      <c r="H40" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I40" t="b">
@@ -1646,22 +1653,22 @@
       <c r="B43" t="b">
         <v>0</v>
       </c>
-      <c r="C43" t="b">
+      <c r="C43" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
       </c>
-      <c r="E43" t="b">
-        <v>1</v>
-      </c>
-      <c r="F43" t="b">
+      <c r="E43" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G43" t="b">
         <v>0</v>
       </c>
-      <c r="H43" t="b">
+      <c r="H43" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I43" t="b">
@@ -1733,22 +1740,22 @@
       <c r="B46" t="b">
         <v>0</v>
       </c>
-      <c r="C46" t="b">
-        <v>1</v>
-      </c>
-      <c r="D46" t="b">
-        <v>1</v>
-      </c>
-      <c r="E46" t="b">
-        <v>1</v>
-      </c>
-      <c r="F46" t="b">
-        <v>1</v>
-      </c>
-      <c r="G46" t="b">
-        <v>1</v>
-      </c>
-      <c r="H46" t="b">
+      <c r="C46" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G46" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I46" t="b">
@@ -1820,25 +1827,721 @@
       <c r="B49" t="b">
         <v>0</v>
       </c>
-      <c r="C49" t="b">
-        <v>0</v>
+      <c r="C49" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
       </c>
-      <c r="E49" t="b">
-        <v>0</v>
-      </c>
-      <c r="F49" t="b">
-        <v>0</v>
+      <c r="E49" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="G49" t="b">
         <v>0</v>
       </c>
-      <c r="H49" t="b">
-        <v>0</v>
+      <c r="H49" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="b">
+        <v>0</v>
+      </c>
+      <c r="C50" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" t="b">
+        <v>0</v>
+      </c>
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="b">
+        <v>0</v>
+      </c>
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" t="b">
+        <v>0</v>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="b">
+        <v>0</v>
+      </c>
+      <c r="C52" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D52" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="b">
+        <v>0</v>
+      </c>
+      <c r="C53" t="b">
+        <v>0</v>
+      </c>
+      <c r="D53" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" t="b">
+        <v>0</v>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="b">
+        <v>0</v>
+      </c>
+      <c r="C54" t="b">
+        <v>0</v>
+      </c>
+      <c r="D54" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" t="b">
+        <v>0</v>
+      </c>
+      <c r="F54" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="b">
+        <v>0</v>
+      </c>
+      <c r="C55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="b">
+        <v>0</v>
+      </c>
+      <c r="C56" t="b">
+        <v>0</v>
+      </c>
+      <c r="D56" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" t="b">
+        <v>0</v>
+      </c>
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="b">
+        <v>0</v>
+      </c>
+      <c r="C57" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="b">
+        <v>0</v>
+      </c>
+      <c r="C58" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D58" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="b">
+        <v>0</v>
+      </c>
+      <c r="C59" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" t="b">
+        <v>0</v>
+      </c>
+      <c r="F59" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="b">
+        <v>0</v>
+      </c>
+      <c r="C60" t="b">
+        <v>0</v>
+      </c>
+      <c r="D60" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" t="b">
+        <v>0</v>
+      </c>
+      <c r="F60" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="b">
+        <v>0</v>
+      </c>
+      <c r="C61" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D61" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G61" t="b">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="b">
+        <v>0</v>
+      </c>
+      <c r="C62" t="b">
+        <v>0</v>
+      </c>
+      <c r="D62" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" t="b">
+        <v>0</v>
+      </c>
+      <c r="F62" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62" t="b">
+        <v>0</v>
+      </c>
+      <c r="I62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="b">
+        <v>0</v>
+      </c>
+      <c r="C63" t="b">
+        <v>0</v>
+      </c>
+      <c r="D63" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" t="b">
+        <v>0</v>
+      </c>
+      <c r="G63" t="b">
+        <v>0</v>
+      </c>
+      <c r="H63" t="b">
+        <v>0</v>
+      </c>
+      <c r="I63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="b">
+        <v>0</v>
+      </c>
+      <c r="C64" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E64" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G64" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H64" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="b">
+        <v>0</v>
+      </c>
+      <c r="C65" t="b">
+        <v>0</v>
+      </c>
+      <c r="D65" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" t="b">
+        <v>0</v>
+      </c>
+      <c r="G65" t="b">
+        <v>0</v>
+      </c>
+      <c r="H65" t="b">
+        <v>0</v>
+      </c>
+      <c r="I65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="b">
+        <v>0</v>
+      </c>
+      <c r="C66" t="b">
+        <v>0</v>
+      </c>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" t="b">
+        <v>0</v>
+      </c>
+      <c r="G66" t="b">
+        <v>0</v>
+      </c>
+      <c r="H66" t="b">
+        <v>0</v>
+      </c>
+      <c r="I66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="b">
+        <v>0</v>
+      </c>
+      <c r="C67" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D67" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G67" t="b">
+        <v>0</v>
+      </c>
+      <c r="H67" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="b">
+        <v>0</v>
+      </c>
+      <c r="C68" t="b">
+        <v>0</v>
+      </c>
+      <c r="D68" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" t="b">
+        <v>0</v>
+      </c>
+      <c r="H68" t="b">
+        <v>0</v>
+      </c>
+      <c r="I68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="b">
+        <v>0</v>
+      </c>
+      <c r="C69" t="b">
+        <v>0</v>
+      </c>
+      <c r="D69" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69" t="b">
+        <v>0</v>
+      </c>
+      <c r="H69" t="b">
+        <v>0</v>
+      </c>
+      <c r="I69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="b">
+        <v>0</v>
+      </c>
+      <c r="C70" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D70" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="b">
+        <v>0</v>
+      </c>
+      <c r="C71" t="b">
+        <v>0</v>
+      </c>
+      <c r="D71" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" t="b">
+        <v>0</v>
+      </c>
+      <c r="F71" t="b">
+        <v>0</v>
+      </c>
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71" t="b">
+        <v>0</v>
+      </c>
+      <c r="I71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="b">
+        <v>0</v>
+      </c>
+      <c r="C72" t="b">
+        <v>0</v>
+      </c>
+      <c r="D72" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" t="b">
+        <v>0</v>
+      </c>
+      <c r="F72" t="b">
+        <v>0</v>
+      </c>
+      <c r="G72" t="b">
+        <v>0</v>
+      </c>
+      <c r="H72" t="b">
+        <v>0</v>
+      </c>
+      <c r="I72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="b">
+        <v>0</v>
+      </c>
+      <c r="C73" t="b">
+        <v>0</v>
+      </c>
+      <c r="D73" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" t="b">
+        <v>0</v>
+      </c>
+      <c r="G73" t="b">
+        <v>0</v>
+      </c>
+      <c r="H73" t="b">
+        <v>0</v>
+      </c>
+      <c r="I73" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>